<commit_message>
updating all files with new INPFC documents
</commit_message>
<xml_diff>
--- a/npmsdd/npmsdd_data_entry_template.xlsx
+++ b/npmsdd/npmsdd_data_entry_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgraham/Sync/Marine Salmon Diet Database/Data entry/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgraham/Sync/Marine Salmon Diet Database/Publication/revised submission/Github/msdd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416D45AC-BE0B-1D48-9803-5573797B2419}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8D77D0-4C60-6144-8EFC-9A525ED4D04C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" xr2:uid="{A228351B-D3D3-3A4B-9B1B-D13362CC00F1}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" xr2:uid="{A228351B-D3D3-3A4B-9B1B-D13362CC00F1}"/>
   </bookViews>
   <sheets>
     <sheet name="sources" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>url</t>
   </si>
   <si>
-    <t>citation_apa</t>
-  </si>
-  <si>
     <t>source_notes</t>
   </si>
   <si>
@@ -415,6 +412,9 @@
   </si>
   <si>
     <t>data_processing_notes</t>
+  </si>
+  <si>
+    <t>citation</t>
   </si>
 </sst>
 </file>
@@ -769,7 +769,7 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -818,19 +818,19 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
+        <v>125</v>
+      </c>
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
+        <v>124</v>
+      </c>
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
-        <v>125</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -850,100 +850,100 @@
   <sheetData>
     <row r="1" spans="1:32">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>27</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>28</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>29</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>30</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>32</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>33</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>34</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>35</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>36</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>37</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>38</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>39</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>40</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>41</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>42</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>43</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>45</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>46</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -966,100 +966,100 @@
   <sheetData>
     <row r="1" spans="1:32">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>27</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>28</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>29</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>30</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>32</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>33</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>34</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>35</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>36</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>37</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>38</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>39</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>40</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>41</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>42</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>43</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>45</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>46</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1082,157 +1082,157 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>53</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>55</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>56</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>57</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>58</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>59</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>60</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>61</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>62</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>63</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>64</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>65</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>66</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>67</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>68</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>69</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>70</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>71</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>72</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>73</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>74</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>75</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>76</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>77</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>78</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>79</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>80</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>81</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>82</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>83</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>84</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>86</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>87</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>88</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>89</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>90</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>91</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>92</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>93</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>94</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>95</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>96</v>
       </c>
-      <c r="AW1" t="s">
-        <v>97</v>
-      </c>
       <c r="AX1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AY1" t="s">
         <v>122</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>123</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1255,163 +1255,163 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>53</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>55</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>56</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>57</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>58</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>59</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>60</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>61</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>62</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>63</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>64</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>65</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>66</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>67</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>68</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>69</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>70</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>71</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>72</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>73</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>74</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>75</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>76</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>77</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>78</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>79</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>80</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>81</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>82</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>83</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>84</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>86</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>87</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>88</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>89</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>90</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>91</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>92</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>93</v>
       </c>
-      <c r="AT1" t="s">
-        <v>94</v>
-      </c>
       <c r="AU1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AW1" t="s">
         <v>100</v>
       </c>
-      <c r="AV1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>101</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>102</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>103</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>104</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>105</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1434,190 +1434,190 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>53</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>55</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>56</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>57</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>58</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>59</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>60</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>61</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>62</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>63</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>64</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>65</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>66</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>67</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>68</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>69</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>70</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>71</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>72</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>73</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>74</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>75</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>76</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>77</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>78</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>79</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>80</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>81</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>82</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>83</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>84</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>86</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>87</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>88</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>89</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>90</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>91</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>92</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>93</v>
       </c>
-      <c r="AT1" t="s">
-        <v>94</v>
-      </c>
       <c r="AU1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AX1" t="s">
         <v>98</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AY1" t="s">
         <v>108</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AZ1" t="s">
+        <v>109</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>110</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>111</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BE1" t="s">
         <v>114</v>
       </c>
-      <c r="AX1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>110</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>111</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>113</v>
-      </c>
-      <c r="BD1" t="s">
+      <c r="BF1" t="s">
         <v>100</v>
       </c>
-      <c r="BE1" t="s">
-        <v>115</v>
-      </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>101</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>102</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>103</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>104</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>105</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1640,85 +1640,85 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>53</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>55</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>56</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>57</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>58</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>59</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>60</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>61</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>62</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>63</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>64</v>
       </c>
-      <c r="Q1" t="s">
-        <v>65</v>
-      </c>
       <c r="R1" t="s">
+        <v>115</v>
+      </c>
+      <c r="S1" t="s">
         <v>116</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>117</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>118</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W1" t="s">
+        <v>100</v>
+      </c>
+      <c r="X1" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB1" t="s">
         <v>119</v>
-      </c>
-      <c r="V1" t="s">
-        <v>121</v>
-      </c>
-      <c r="W1" t="s">
-        <v>101</v>
-      </c>
-      <c r="X1" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>103</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>